<commit_message>
Cargando datos finales para entrega1 previo a presentación
</commit_message>
<xml_diff>
--- a/df_total_e1.xlsx
+++ b/df_total_e1.xlsx
@@ -26156,7 +26156,7 @@
     </row>
     <row r="552">
       <c r="A552" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B552" t="inlineStr">
         <is>
@@ -26190,7 +26190,7 @@
       </c>
       <c r="H552" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I552" t="inlineStr">
@@ -26201,7 +26201,7 @@
     </row>
     <row r="553">
       <c r="A553" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B553" t="inlineStr">
         <is>
@@ -26235,7 +26235,7 @@
       </c>
       <c r="H553" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I553" t="inlineStr">
@@ -26246,7 +26246,7 @@
     </row>
     <row r="554">
       <c r="A554" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B554" t="inlineStr">
         <is>
@@ -26280,7 +26280,7 @@
       </c>
       <c r="H554" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I554" t="inlineStr">
@@ -26291,7 +26291,7 @@
     </row>
     <row r="555">
       <c r="A555" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B555" t="inlineStr">
         <is>
@@ -26325,7 +26325,7 @@
       </c>
       <c r="H555" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I555" t="inlineStr">
@@ -26336,7 +26336,7 @@
     </row>
     <row r="556">
       <c r="A556" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B556" t="inlineStr">
         <is>
@@ -26370,7 +26370,7 @@
       </c>
       <c r="H556" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I556" t="inlineStr">
@@ -26381,7 +26381,7 @@
     </row>
     <row r="557">
       <c r="A557" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B557" t="inlineStr">
         <is>
@@ -26413,7 +26413,7 @@
       </c>
       <c r="H557" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I557" t="inlineStr">
@@ -26424,7 +26424,7 @@
     </row>
     <row r="558">
       <c r="A558" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B558" t="inlineStr">
         <is>
@@ -26458,7 +26458,7 @@
       </c>
       <c r="H558" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I558" t="inlineStr">
@@ -26469,7 +26469,7 @@
     </row>
     <row r="559">
       <c r="A559" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B559" t="inlineStr">
         <is>
@@ -26503,7 +26503,7 @@
       </c>
       <c r="H559" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I559" t="inlineStr">
@@ -26514,7 +26514,7 @@
     </row>
     <row r="560">
       <c r="A560" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B560" t="inlineStr">
         <is>
@@ -26548,7 +26548,7 @@
       </c>
       <c r="H560" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I560" t="inlineStr">
@@ -26559,7 +26559,7 @@
     </row>
     <row r="561">
       <c r="A561" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B561" t="inlineStr">
         <is>
@@ -26593,7 +26593,7 @@
       </c>
       <c r="H561" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I561" t="inlineStr">
@@ -26604,7 +26604,7 @@
     </row>
     <row r="562">
       <c r="A562" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B562" t="inlineStr">
         <is>
@@ -26636,7 +26636,7 @@
       </c>
       <c r="H562" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I562" t="inlineStr">
@@ -26647,7 +26647,7 @@
     </row>
     <row r="563">
       <c r="A563" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B563" t="inlineStr">
         <is>
@@ -26681,7 +26681,7 @@
       </c>
       <c r="H563" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I563" t="inlineStr">
@@ -26692,7 +26692,7 @@
     </row>
     <row r="564">
       <c r="A564" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B564" t="inlineStr">
         <is>
@@ -26726,7 +26726,7 @@
       </c>
       <c r="H564" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I564" t="inlineStr">
@@ -26737,7 +26737,7 @@
     </row>
     <row r="565">
       <c r="A565" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B565" t="inlineStr">
         <is>
@@ -26771,7 +26771,7 @@
       </c>
       <c r="H565" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I565" t="inlineStr">
@@ -26782,7 +26782,7 @@
     </row>
     <row r="566">
       <c r="A566" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B566" t="inlineStr">
         <is>
@@ -26816,7 +26816,7 @@
       </c>
       <c r="H566" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I566" t="inlineStr">
@@ -26827,7 +26827,7 @@
     </row>
     <row r="567">
       <c r="A567" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B567" t="inlineStr">
         <is>
@@ -26859,7 +26859,7 @@
       </c>
       <c r="H567" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I567" t="inlineStr">
@@ -26870,7 +26870,7 @@
     </row>
     <row r="568">
       <c r="A568" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B568" t="inlineStr">
         <is>
@@ -26904,7 +26904,7 @@
       </c>
       <c r="H568" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I568" t="inlineStr">
@@ -26915,7 +26915,7 @@
     </row>
     <row r="569">
       <c r="A569" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B569" t="inlineStr">
         <is>
@@ -26949,7 +26949,7 @@
       </c>
       <c r="H569" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I569" t="inlineStr">
@@ -26960,7 +26960,7 @@
     </row>
     <row r="570">
       <c r="A570" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B570" t="inlineStr">
         <is>
@@ -26994,7 +26994,7 @@
       </c>
       <c r="H570" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I570" t="inlineStr">
@@ -27005,7 +27005,7 @@
     </row>
     <row r="571">
       <c r="A571" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B571" t="inlineStr">
         <is>
@@ -27039,7 +27039,7 @@
       </c>
       <c r="H571" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I571" t="inlineStr">
@@ -27050,7 +27050,7 @@
     </row>
     <row r="572">
       <c r="A572" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B572" t="inlineStr">
         <is>
@@ -27082,7 +27082,7 @@
       </c>
       <c r="H572" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I572" t="inlineStr">
@@ -27093,7 +27093,7 @@
     </row>
     <row r="573">
       <c r="A573" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B573" t="inlineStr">
         <is>
@@ -27127,7 +27127,7 @@
       </c>
       <c r="H573" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I573" t="inlineStr">
@@ -27138,7 +27138,7 @@
     </row>
     <row r="574">
       <c r="A574" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B574" t="inlineStr">
         <is>
@@ -27172,7 +27172,7 @@
       </c>
       <c r="H574" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I574" t="inlineStr">
@@ -27183,7 +27183,7 @@
     </row>
     <row r="575">
       <c r="A575" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B575" t="inlineStr">
         <is>
@@ -27217,7 +27217,7 @@
       </c>
       <c r="H575" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I575" t="inlineStr">
@@ -27228,7 +27228,7 @@
     </row>
     <row r="576">
       <c r="A576" t="n">
-        <v>0</v>
+        <v>30000120847</v>
       </c>
       <c r="B576" t="inlineStr">
         <is>
@@ -27262,7 +27262,7 @@
       </c>
       <c r="H576" t="inlineStr">
         <is>
-          <t>0_MaAl</t>
+          <t>30000120847_MaAl</t>
         </is>
       </c>
       <c r="I576" t="inlineStr">
@@ -34275,7 +34275,7 @@
     </row>
     <row r="727">
       <c r="A727" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B727" t="inlineStr">
         <is>
@@ -34309,7 +34309,7 @@
       </c>
       <c r="H727" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I727" t="inlineStr">
@@ -34320,7 +34320,7 @@
     </row>
     <row r="728">
       <c r="A728" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B728" t="inlineStr">
         <is>
@@ -34354,7 +34354,7 @@
       </c>
       <c r="H728" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I728" t="inlineStr">
@@ -34365,7 +34365,7 @@
     </row>
     <row r="729">
       <c r="A729" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B729" t="inlineStr">
         <is>
@@ -34399,7 +34399,7 @@
       </c>
       <c r="H729" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I729" t="inlineStr">
@@ -34410,7 +34410,7 @@
     </row>
     <row r="730">
       <c r="A730" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B730" t="inlineStr">
         <is>
@@ -34444,7 +34444,7 @@
       </c>
       <c r="H730" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I730" t="inlineStr">
@@ -34455,7 +34455,7 @@
     </row>
     <row r="731">
       <c r="A731" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B731" t="inlineStr">
         <is>
@@ -34489,7 +34489,7 @@
       </c>
       <c r="H731" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I731" t="inlineStr">
@@ -34500,7 +34500,7 @@
     </row>
     <row r="732">
       <c r="A732" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B732" t="inlineStr">
         <is>
@@ -34532,7 +34532,7 @@
       </c>
       <c r="H732" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I732" t="inlineStr">
@@ -34543,7 +34543,7 @@
     </row>
     <row r="733">
       <c r="A733" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B733" t="inlineStr">
         <is>
@@ -34577,7 +34577,7 @@
       </c>
       <c r="H733" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I733" t="inlineStr">
@@ -34588,7 +34588,7 @@
     </row>
     <row r="734">
       <c r="A734" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B734" t="inlineStr">
         <is>
@@ -34622,7 +34622,7 @@
       </c>
       <c r="H734" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I734" t="inlineStr">
@@ -34633,7 +34633,7 @@
     </row>
     <row r="735">
       <c r="A735" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B735" t="inlineStr">
         <is>
@@ -34667,7 +34667,7 @@
       </c>
       <c r="H735" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I735" t="inlineStr">
@@ -34678,7 +34678,7 @@
     </row>
     <row r="736">
       <c r="A736" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B736" t="inlineStr">
         <is>
@@ -34712,7 +34712,7 @@
       </c>
       <c r="H736" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I736" t="inlineStr">
@@ -34723,7 +34723,7 @@
     </row>
     <row r="737">
       <c r="A737" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B737" t="inlineStr">
         <is>
@@ -34755,7 +34755,7 @@
       </c>
       <c r="H737" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I737" t="inlineStr">
@@ -34766,7 +34766,7 @@
     </row>
     <row r="738">
       <c r="A738" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B738" t="inlineStr">
         <is>
@@ -34800,7 +34800,7 @@
       </c>
       <c r="H738" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I738" t="inlineStr">
@@ -34811,7 +34811,7 @@
     </row>
     <row r="739">
       <c r="A739" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B739" t="inlineStr">
         <is>
@@ -34845,7 +34845,7 @@
       </c>
       <c r="H739" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I739" t="inlineStr">
@@ -34856,7 +34856,7 @@
     </row>
     <row r="740">
       <c r="A740" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B740" t="inlineStr">
         <is>
@@ -34890,7 +34890,7 @@
       </c>
       <c r="H740" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I740" t="inlineStr">
@@ -34901,7 +34901,7 @@
     </row>
     <row r="741">
       <c r="A741" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B741" t="inlineStr">
         <is>
@@ -34935,7 +34935,7 @@
       </c>
       <c r="H741" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I741" t="inlineStr">
@@ -34946,7 +34946,7 @@
     </row>
     <row r="742">
       <c r="A742" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B742" t="inlineStr">
         <is>
@@ -34978,7 +34978,7 @@
       </c>
       <c r="H742" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I742" t="inlineStr">
@@ -34989,7 +34989,7 @@
     </row>
     <row r="743">
       <c r="A743" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B743" t="inlineStr">
         <is>
@@ -35023,7 +35023,7 @@
       </c>
       <c r="H743" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I743" t="inlineStr">
@@ -35034,7 +35034,7 @@
     </row>
     <row r="744">
       <c r="A744" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B744" t="inlineStr">
         <is>
@@ -35068,7 +35068,7 @@
       </c>
       <c r="H744" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I744" t="inlineStr">
@@ -35079,7 +35079,7 @@
     </row>
     <row r="745">
       <c r="A745" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B745" t="inlineStr">
         <is>
@@ -35113,7 +35113,7 @@
       </c>
       <c r="H745" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I745" t="inlineStr">
@@ -35124,7 +35124,7 @@
     </row>
     <row r="746">
       <c r="A746" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B746" t="inlineStr">
         <is>
@@ -35158,7 +35158,7 @@
       </c>
       <c r="H746" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I746" t="inlineStr">
@@ -35169,7 +35169,7 @@
     </row>
     <row r="747">
       <c r="A747" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B747" t="inlineStr">
         <is>
@@ -35201,7 +35201,7 @@
       </c>
       <c r="H747" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I747" t="inlineStr">
@@ -35212,7 +35212,7 @@
     </row>
     <row r="748">
       <c r="A748" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B748" t="inlineStr">
         <is>
@@ -35246,7 +35246,7 @@
       </c>
       <c r="H748" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I748" t="inlineStr">
@@ -35257,7 +35257,7 @@
     </row>
     <row r="749">
       <c r="A749" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B749" t="inlineStr">
         <is>
@@ -35291,7 +35291,7 @@
       </c>
       <c r="H749" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I749" t="inlineStr">
@@ -35302,7 +35302,7 @@
     </row>
     <row r="750">
       <c r="A750" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B750" t="inlineStr">
         <is>
@@ -35336,7 +35336,7 @@
       </c>
       <c r="H750" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I750" t="inlineStr">
@@ -35347,7 +35347,7 @@
     </row>
     <row r="751">
       <c r="A751" t="n">
-        <v>0</v>
+        <v>30000096203</v>
       </c>
       <c r="B751" t="inlineStr">
         <is>
@@ -35381,7 +35381,7 @@
       </c>
       <c r="H751" t="inlineStr">
         <is>
-          <t>0_MaPa</t>
+          <t>30000096203_MaPa</t>
         </is>
       </c>
       <c r="I751" t="inlineStr">

</xml_diff>